<commit_message>
add obj prop import candidates + minor method restructure
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
+++ b/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BF044D-3740-4F3B-B7AA-4DC18D0BBEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D068C390-222B-4E11-A13F-AB98A6F91607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="21760" windowHeight="13840" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="amber+cpptraj" sheetId="1" r:id="rId1"/>
@@ -14520,9 +14520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF52D84-4AB6-470B-8703-41185DC33D82}">
   <dimension ref="A1:L1669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A615" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F615" sqref="F615"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J525" sqref="J525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14530,7 +14530,7 @@
     <col min="1" max="1" width="10.90625" customWidth="1"/>
     <col min="2" max="3" width="6.6328125" customWidth="1"/>
     <col min="4" max="5" width="15.6328125" customWidth="1"/>
-    <col min="6" max="6" width="117.6328125" customWidth="1"/>
+    <col min="6" max="6" width="55.54296875" customWidth="1"/>
     <col min="7" max="7" width="36.08984375" customWidth="1"/>
     <col min="8" max="8" width="26.26953125" customWidth="1"/>
     <col min="9" max="9" width="35.08984375" customWidth="1"/>

</xml_diff>

<commit_message>
update cpptraj/amber sheet wrt method terms omission/addition
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
+++ b/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D068C390-222B-4E11-A13F-AB98A6F91607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB4480D-F7F1-420A-8F83-EDEE46104C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="21760" windowHeight="13840" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
+    <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="amber+cpptraj" sheetId="1" r:id="rId1"/>
@@ -138,12 +138,459 @@
         </r>
       </text>
     </comment>
+    <comment ref="G903" authorId="0" shapeId="0" xr:uid="{5DF96921-46E6-4462-9FCA-39E3878D8CE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+subclass of SAS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G941" authorId="0" shapeId="0" xr:uid="{424E9F15-EDE9-423F-B6E4-365252CC7EA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+the parameter version existed - but not the GaMD itself.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G946" authorId="0" shapeId="0" xr:uid="{BC57590D-5EE7-4BAB-B980-14A9F9307EDB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+need to be moved to algorithm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G950" authorId="0" shapeId="0" xr:uid="{D54F4BDF-1B13-4EA3-B71F-A0B961875F91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as replica-exchange (MOLSIM:000858).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G954" authorId="0" shapeId="0" xr:uid="{D48EE567-1A4F-449F-A45B-CD52FA819E6B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+But could be addes as a subclass of replica-exchange MD?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G971" authorId="0" shapeId="0" xr:uid="{E097974D-9ACB-4268-93E3-B9F760374D04}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+..as accelerated MD parmeter, but aMD itself does not exist yet.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1002" authorId="0" shapeId="0" xr:uid="{4A2C8633-23A9-404D-8AE8-E479725DE292}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as free energy perturbation (MOLSIM:000266). This is a synonym.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1005" authorId="0" shapeId="0" xr:uid="{BB0B867A-8363-4ABF-853A-D4F72CB2F234}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ sampling method. ALREADY EXISTS as string method (MOLSIM:000860). This is a specific type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1012" authorId="0" shapeId="0" xr:uid="{F16A2149-AF7D-4E6C-AFAC-BF27D2DCD32C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:may need recheck if we should omit this</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1013" authorId="0" shapeId="0" xr:uid="{1E587E57-A4DF-41E7-A26E-A60BB1A07BA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as secondary structure* (MOLSIM:000981). Should be renamed to secondary structure assignment.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1060" authorId="0" shapeId="0" xr:uid="{E02BAEFF-6E08-436F-9516-2E1C9FC2EAFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as energy analysis (MOLSIM:000950).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1070" authorId="0" shapeId="0" xr:uid="{3D1D733E-A9FE-4F38-AB25-CD33A6005C7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+evaluate whether this should be a  charge model instead.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1098" authorId="0" shapeId="0" xr:uid="{C409DC2E-9488-4C32-AC58-597365D51239}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as restraint electrostatic potential (MOLSIM:000206). This is a specific implementation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1101" authorId="0" shapeId="0" xr:uid="{ABA5314A-2B67-4BA1-919C-9384587A4AEC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+these both could belong to model</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1103" authorId="0" shapeId="0" xr:uid="{B887937A-3043-413F-8D17-EFB3337AF9EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as restraint electrostatic potential (MOLSIM:000206). This is a synonym.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1110" authorId="0" shapeId="0" xr:uid="{7D2F40F0-2BEE-4545-BF15-8A21D06FB2C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Gaussian fluctuation free energy method</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1124" authorId="0" shapeId="0" xr:uid="{D33E1B7F-E1EB-4C07-9153-64D5F65A3B64}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as steered dynamics (MOLSIM:000859). Should probably renamed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1131" authorId="0" shapeId="0" xr:uid="{8300FFEB-94EB-48BC-9812-F5A4C05C414D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as constant redox potential molecular dynamics. This is a synonym.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1133" authorId="0" shapeId="0" xr:uid="{54C3FF1B-0841-40EC-9A3A-27FBBB90F3E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ALREADY EXISTS as energy decomposition analysis (MOLSIM:000606).</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10583" uniqueCount="4663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10891" uniqueCount="4784">
   <si>
     <t>skip? (-=yes)</t>
   </si>
@@ -14132,13 +14579,376 @@
   </si>
   <si>
     <t>distance matrix file</t>
+  </si>
+  <si>
+    <t>ion concentration calculation method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welch's T-test </t>
+  </si>
+  <si>
+    <t>ex</t>
+  </si>
+  <si>
+    <t>R6 integration/r-6 weighted distance averaging</t>
+  </si>
+  <si>
+    <t>well-tempered adaptively biased molecular dynamics</t>
+  </si>
+  <si>
+    <t>ZLM density fitting</t>
+  </si>
+  <si>
+    <t>Z-matrix parameterization method</t>
+  </si>
+  <si>
+    <t>force interpolation method</t>
+  </si>
+  <si>
+    <t>adaptive thermostat</t>
+  </si>
+  <si>
+    <t>Mulliken Ewald summation</t>
+  </si>
+  <si>
+    <t>QM-QM derivative calculation method</t>
+  </si>
+  <si>
+    <t>QM Ewald treatment</t>
+  </si>
+  <si>
+    <t>hot spot adaptive QM/MM</t>
+  </si>
+  <si>
+    <t>isotropic periodic sum method</t>
+  </si>
+  <si>
+    <t>semi-isotropic pressure scaling barostat</t>
+  </si>
+  <si>
+    <t>direct sum Coulomb method</t>
+  </si>
+  <si>
+    <t>self-guided Langevin dynamics</t>
+  </si>
+  <si>
+    <t>generalized Langevin equation self-guided Langevin dynamics</t>
+  </si>
+  <si>
+    <t>ligand Gaussian accelerated molecular dynamics</t>
+  </si>
+  <si>
+    <t>ligand Gaussian accelerated molecular dynamics 3</t>
+  </si>
+  <si>
+    <t>dual-boost ligand Gaussian accelerated molecular dynamics</t>
+  </si>
+  <si>
+    <t>peptide Gaussian accelerated molecular dynamics</t>
+  </si>
+  <si>
+    <t>dual-boost peptide Gaussian accelerated molecular dynamics</t>
+  </si>
+  <si>
+    <t>protein-protein interaction Gaussian accelerated molecular dynamics</t>
+  </si>
+  <si>
+    <t>dual-boost protein-protein interaction Gaussian accelerated</t>
+  </si>
+  <si>
+    <t>multiply-targeted molecular dynamics</t>
+  </si>
+  <si>
+    <t>partial nudged elastic band</t>
+  </si>
+  <si>
+    <t>XMIN minimization</t>
+  </si>
+  <si>
+    <t>lambda-scheduling free energy method</t>
+  </si>
+  <si>
+    <t>hybrid solvent replica-exchange molecular dynamics</t>
+  </si>
+  <si>
+    <t>reservoir replica-exchange molecular dynamics</t>
+  </si>
+  <si>
+    <t>replica-exchange umbrella sampling</t>
+  </si>
+  <si>
+    <t>replica-exchange with arbitrary degree of freedom</t>
+  </si>
+  <si>
+    <t>EMIL free energy method</t>
+  </si>
+  <si>
+    <t>continuous constant pH molecular dynamics</t>
+  </si>
+  <si>
+    <t>lambda-dynamics free energy method</t>
+  </si>
+  <si>
+    <t>_PME continuous constant pH molecular dynamics</t>
+  </si>
+  <si>
+    <t>variational free energy profile method</t>
+  </si>
+  <si>
+    <t>weighted thermodynamic perturbation theory</t>
+  </si>
+  <si>
+    <t>generalized weighted thermodynamic perturbation theory</t>
+  </si>
+  <si>
+    <t>multidimensional replica-exchange molecular dynamics</t>
+  </si>
+  <si>
+    <t>grid inhomogeneous solvation theory</t>
+  </si>
+  <si>
+    <t>kernel modified molecular dynamics</t>
+  </si>
+  <si>
+    <t>isotropically distributed ensemble analysis</t>
+  </si>
+  <si>
+    <t>isotropic reorientational eigenmode dynamics</t>
+  </si>
+  <si>
+    <t>nucleic acid structure analysis</t>
+  </si>
+  <si>
+    <t>time-lagged independent component analysis</t>
+  </si>
+  <si>
+    <t>wavelet analysis feature extraction</t>
+  </si>
+  <si>
+    <t>path integral molecular dynamics</t>
+  </si>
+  <si>
+    <t>spatial properties of activity by mapping</t>
+  </si>
+  <si>
+    <t>Lennard-Jones particle mesh Ewald</t>
+  </si>
+  <si>
+    <t>Altona &amp; Sundaralingam pucker analysis</t>
+  </si>
+  <si>
+    <t>Cremer &amp; Pople pucker analysis</t>
+  </si>
+  <si>
+    <t>hydrogen bond analysis</t>
+  </si>
+  <si>
+    <t>native contact analysis</t>
+  </si>
+  <si>
+    <t>Forster resonance energy transfer</t>
+  </si>
+  <si>
+    <t>CHELPG charge analysis</t>
+  </si>
+  <si>
+    <t>Connolly surface calculation</t>
+  </si>
+  <si>
+    <t>covariance matrix calculation</t>
+  </si>
+  <si>
+    <t>2D root-mean-square deviation analysis</t>
+  </si>
+  <si>
+    <t>lipid SCD order parameter calculation</t>
+  </si>
+  <si>
+    <t>3D reference interaction site model</t>
+  </si>
+  <si>
+    <t>adaptive solvent QM/MM</t>
+  </si>
+  <si>
+    <t>iterative polarizable charge method</t>
+  </si>
+  <si>
+    <t>mechanical embedding QM/MM</t>
+  </si>
+  <si>
+    <t>QM generalized Born treatment</t>
+  </si>
+  <si>
+    <t>time-averaged restraint simulation</t>
+  </si>
+  <si>
+    <t>Gaussian fluctuation free energy method</t>
+  </si>
+  <si>
+    <t>PC+ correction method</t>
+  </si>
+  <si>
+    <t>universal correction method</t>
+  </si>
+  <si>
+    <t>density-functional based tight-binding</t>
+  </si>
+  <si>
+    <t>self-consistent-charge density-functional based tight-binding</t>
+  </si>
+  <si>
+    <t>third-order self-consistent-charge density-functional based tight-binding</t>
+  </si>
+  <si>
+    <t>density functional theory</t>
+  </si>
+  <si>
+    <t>QM/MM simulation</t>
+  </si>
+  <si>
+    <t>electrostatic embedding QM/MM</t>
+  </si>
+  <si>
+    <t>QM/MM Ewald summation</t>
+  </si>
+  <si>
+    <t>multilayer QM/MM</t>
+  </si>
+  <si>
+    <t>difference-based adaptive solvation QM/MM</t>
+  </si>
+  <si>
+    <t>adaptive buffered force-mixing QM/MM</t>
+  </si>
+  <si>
+    <t>semi-empirical Born-Oppenheimer molecular dynamics</t>
+  </si>
+  <si>
+    <t>hybrid ReaxFF/AMBER molecular dynamics</t>
+  </si>
+  <si>
+    <t>charge equilibration method</t>
+  </si>
+  <si>
+    <t>electronegativity equalization method</t>
+  </si>
+  <si>
+    <t>Gaussian-shaped constraint simulation</t>
+  </si>
+  <si>
+    <t>ABCG2 charge method</t>
+  </si>
+  <si>
+    <t>empirical metal center parameterization</t>
+  </si>
+  <si>
+    <t>BAR/PBSA method</t>
+  </si>
+  <si>
+    <t>hybrid solvent MM-PBSA</t>
+  </si>
+  <si>
+    <t>kinetic map analysis</t>
+  </si>
+  <si>
+    <t>commute map analysis</t>
+  </si>
+  <si>
+    <t>constant pH molecular dynamics</t>
+  </si>
+  <si>
+    <t>energy decomposition analysis</t>
+  </si>
+  <si>
+    <t>entropic decomposition analysis</t>
+  </si>
+  <si>
+    <t>molecular reconstruction from distribution functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polar decomposition analysis </t>
+  </si>
+  <si>
+    <t>replica-exchange free energy perturbation</t>
+  </si>
+  <si>
+    <t>constant redox potential molecular dynamics</t>
+  </si>
+  <si>
+    <t>ensemble trajectory analysis</t>
+  </si>
+  <si>
+    <t>grid binning analysis</t>
+  </si>
+  <si>
+    <t>periodic boundary imaging</t>
+  </si>
+  <si>
+    <t>LES trajectory splitting</t>
+  </si>
+  <si>
+    <t>structure modification method</t>
+  </si>
+  <si>
+    <t>ion randomization method</t>
+  </si>
+  <si>
+    <t>cell replication method</t>
+  </si>
+  <si>
+    <t>coordinate scaling method</t>
+  </si>
+  <si>
+    <t>velocity assignment method</t>
+  </si>
+  <si>
+    <t>volumetric map generation</t>
+  </si>
+  <si>
+    <t>topology stripping method</t>
+  </si>
+  <si>
+    <t>force field parameter update method</t>
+  </si>
+  <si>
+    <t>average structure calculation</t>
+  </si>
+  <si>
+    <t>coordinate centering</t>
+  </si>
+  <si>
+    <t>closest solvent analysis</t>
+  </si>
+  <si>
+    <t>trajectory frame filtering</t>
+  </si>
+  <si>
+    <t>atom order fixing</t>
+  </si>
+  <si>
+    <t>image bond fixing</t>
+  </si>
+  <si>
+    <t>atom selection method</t>
+  </si>
+  <si>
+    <t>vector analysis</t>
+  </si>
+  <si>
+    <t>atom remapping method</t>
+  </si>
+  <si>
+    <t>coordinate rotation method</t>
+  </si>
+  <si>
+    <t>running average calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14164,6 +14974,40 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF1A1C1E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF1A1C1E"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -14198,12 +15042,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14520,9 +15368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF52D84-4AB6-470B-8703-41185DC33D82}">
   <dimension ref="A1:L1669"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J525" sqref="J525"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1026" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1196" sqref="G1196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39340,6 +40188,9 @@
       <c r="C888">
         <v>11</v>
       </c>
+      <c r="G888" t="s">
+        <v>1842</v>
+      </c>
       <c r="H888" t="s">
         <v>1842</v>
       </c>
@@ -39366,6 +40217,9 @@
       <c r="C889">
         <v>275</v>
       </c>
+      <c r="G889" s="5" t="s">
+        <v>443</v>
+      </c>
       <c r="H889" t="s">
         <v>1845</v>
       </c>
@@ -39392,6 +40246,9 @@
       <c r="C890">
         <v>318</v>
       </c>
+      <c r="G890" t="s">
+        <v>4663</v>
+      </c>
       <c r="H890" t="s">
         <v>1848</v>
       </c>
@@ -39418,6 +40275,9 @@
       <c r="C891">
         <v>356</v>
       </c>
+      <c r="G891" t="s">
+        <v>1850</v>
+      </c>
       <c r="H891" t="s">
         <v>1850</v>
       </c>
@@ -39444,6 +40304,9 @@
       <c r="C892">
         <v>486</v>
       </c>
+      <c r="G892" t="s">
+        <v>1853</v>
+      </c>
       <c r="H892" t="s">
         <v>1853</v>
       </c>
@@ -39470,6 +40333,9 @@
       <c r="C893">
         <v>496</v>
       </c>
+      <c r="G893" t="s">
+        <v>1856</v>
+      </c>
       <c r="H893" t="s">
         <v>1856</v>
       </c>
@@ -39496,6 +40362,9 @@
       <c r="C894">
         <v>630</v>
       </c>
+      <c r="G894" t="s">
+        <v>1859</v>
+      </c>
       <c r="H894" t="s">
         <v>1859</v>
       </c>
@@ -39522,6 +40391,9 @@
       <c r="C895">
         <v>1001</v>
       </c>
+      <c r="G895" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="H895" t="s">
         <v>1862</v>
       </c>
@@ -39548,6 +40420,9 @@
       <c r="C896">
         <v>1013</v>
       </c>
+      <c r="G896" t="s">
+        <v>1865</v>
+      </c>
       <c r="H896" t="s">
         <v>1865</v>
       </c>
@@ -39574,6 +40449,9 @@
       <c r="C897">
         <v>1014</v>
       </c>
+      <c r="G897" t="s">
+        <v>1867</v>
+      </c>
       <c r="H897" t="s">
         <v>1867</v>
       </c>
@@ -39600,6 +40478,9 @@
       <c r="C898">
         <v>1497</v>
       </c>
+      <c r="G898" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="H898" t="s">
         <v>1869</v>
       </c>
@@ -39626,6 +40507,9 @@
       <c r="C899">
         <v>1498</v>
       </c>
+      <c r="G899" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="H899" t="s">
         <v>1871</v>
       </c>
@@ -39652,6 +40536,9 @@
       <c r="C900">
         <v>1540</v>
       </c>
+      <c r="G900" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="H900" t="s">
         <v>1873</v>
       </c>
@@ -39678,6 +40565,9 @@
       <c r="C901">
         <v>1541</v>
       </c>
+      <c r="G901" s="5" t="s">
+        <v>525</v>
+      </c>
       <c r="H901" t="s">
         <v>1875</v>
       </c>
@@ -39704,6 +40594,9 @@
       <c r="C902">
         <v>1646</v>
       </c>
+      <c r="G902" s="3" t="s">
+        <v>4664</v>
+      </c>
       <c r="H902" t="s">
         <v>1877</v>
       </c>
@@ -39730,6 +40623,9 @@
       <c r="C903">
         <v>1656</v>
       </c>
+      <c r="G903" t="s">
+        <v>1880</v>
+      </c>
       <c r="H903" t="s">
         <v>1880</v>
       </c>
@@ -39756,6 +40652,9 @@
       <c r="C904">
         <v>1668</v>
       </c>
+      <c r="G904" s="6" t="s">
+        <v>1883</v>
+      </c>
       <c r="H904" t="s">
         <v>1883</v>
       </c>
@@ -39782,6 +40681,9 @@
       <c r="C905">
         <v>1669</v>
       </c>
+      <c r="G905" t="s">
+        <v>1886</v>
+      </c>
       <c r="H905" t="s">
         <v>1886</v>
       </c>
@@ -39807,6 +40709,9 @@
       </c>
       <c r="C906">
         <v>1672</v>
+      </c>
+      <c r="G906" t="s">
+        <v>1889</v>
       </c>
       <c r="H906" t="s">
         <v>1889</v>
@@ -39834,6 +40739,9 @@
       <c r="C907">
         <v>126</v>
       </c>
+      <c r="G907" s="5" t="s">
+        <v>443</v>
+      </c>
       <c r="H907" t="s">
         <v>3615</v>
       </c>
@@ -39860,6 +40768,9 @@
       <c r="C908">
         <v>129</v>
       </c>
+      <c r="G908" t="s">
+        <v>443</v>
+      </c>
       <c r="H908" t="s">
         <v>3624</v>
       </c>
@@ -39886,6 +40797,9 @@
       <c r="C909">
         <v>131</v>
       </c>
+      <c r="G909" t="s">
+        <v>443</v>
+      </c>
       <c r="H909" t="s">
         <v>3630</v>
       </c>
@@ -39912,6 +40826,9 @@
       <c r="C910">
         <v>132</v>
       </c>
+      <c r="G910" t="s">
+        <v>443</v>
+      </c>
       <c r="H910" t="s">
         <v>3633</v>
       </c>
@@ -39938,6 +40855,9 @@
       <c r="C911">
         <v>148</v>
       </c>
+      <c r="G911" t="s">
+        <v>443</v>
+      </c>
       <c r="H911" t="s">
         <v>3679</v>
       </c>
@@ -39964,6 +40884,9 @@
       <c r="C912">
         <v>150</v>
       </c>
+      <c r="G912" t="s">
+        <v>443</v>
+      </c>
       <c r="H912" t="s">
         <v>3685</v>
       </c>
@@ -39990,6 +40913,9 @@
       <c r="C913">
         <v>151</v>
       </c>
+      <c r="G913" t="s">
+        <v>443</v>
+      </c>
       <c r="H913" t="s">
         <v>3688</v>
       </c>
@@ -40016,6 +40942,9 @@
       <c r="C914">
         <v>152</v>
       </c>
+      <c r="G914" t="s">
+        <v>443</v>
+      </c>
       <c r="H914" t="s">
         <v>3691</v>
       </c>
@@ -40042,6 +40971,9 @@
       <c r="C915">
         <v>154</v>
       </c>
+      <c r="G915" t="s">
+        <v>443</v>
+      </c>
       <c r="H915" t="s">
         <v>3697</v>
       </c>
@@ -40068,6 +41000,9 @@
       <c r="C916">
         <v>168</v>
       </c>
+      <c r="G916" t="s">
+        <v>443</v>
+      </c>
       <c r="H916" t="s">
         <v>3740</v>
       </c>
@@ -40094,6 +41029,9 @@
       <c r="C917">
         <v>169</v>
       </c>
+      <c r="G917" t="s">
+        <v>443</v>
+      </c>
       <c r="H917" t="s">
         <v>3743</v>
       </c>
@@ -40120,6 +41058,9 @@
       <c r="C918">
         <v>181</v>
       </c>
+      <c r="G918" t="s">
+        <v>443</v>
+      </c>
       <c r="H918" t="s">
         <v>3779</v>
       </c>
@@ -40146,6 +41087,9 @@
       <c r="C919">
         <v>182</v>
       </c>
+      <c r="G919" t="s">
+        <v>443</v>
+      </c>
       <c r="H919" t="s">
         <v>3782</v>
       </c>
@@ -40172,6 +41116,9 @@
       <c r="C920">
         <v>185</v>
       </c>
+      <c r="G920" t="s">
+        <v>443</v>
+      </c>
       <c r="H920" t="s">
         <v>3791</v>
       </c>
@@ -40198,6 +41145,9 @@
       <c r="C921">
         <v>186</v>
       </c>
+      <c r="G921" t="s">
+        <v>443</v>
+      </c>
       <c r="H921" t="s">
         <v>3794</v>
       </c>
@@ -40224,6 +41174,9 @@
       <c r="C922">
         <v>190</v>
       </c>
+      <c r="G922" t="s">
+        <v>443</v>
+      </c>
       <c r="H922" t="s">
         <v>3806</v>
       </c>
@@ -40250,6 +41203,9 @@
       <c r="C923">
         <v>192</v>
       </c>
+      <c r="G923" t="s">
+        <v>443</v>
+      </c>
       <c r="H923" t="s">
         <v>3811</v>
       </c>
@@ -40276,6 +41232,9 @@
       <c r="C924">
         <v>193</v>
       </c>
+      <c r="G924" t="s">
+        <v>443</v>
+      </c>
       <c r="H924" t="s">
         <v>3814</v>
       </c>
@@ -40302,6 +41261,9 @@
       <c r="C925">
         <v>196</v>
       </c>
+      <c r="G925" t="s">
+        <v>443</v>
+      </c>
       <c r="H925" t="s">
         <v>3823</v>
       </c>
@@ -40328,6 +41290,9 @@
       <c r="C926">
         <v>198</v>
       </c>
+      <c r="G926" t="s">
+        <v>443</v>
+      </c>
       <c r="H926" t="s">
         <v>3827</v>
       </c>
@@ -40354,6 +41319,9 @@
       <c r="C927">
         <v>219</v>
       </c>
+      <c r="G927" t="s">
+        <v>443</v>
+      </c>
       <c r="H927" t="s">
         <v>3891</v>
       </c>
@@ -40380,6 +41348,9 @@
       <c r="C928">
         <v>419</v>
       </c>
+      <c r="G928" t="s">
+        <v>443</v>
+      </c>
       <c r="H928" t="s">
         <v>4433</v>
       </c>
@@ -40406,6 +41377,9 @@
       <c r="C929">
         <v>420</v>
       </c>
+      <c r="G929" t="s">
+        <v>443</v>
+      </c>
       <c r="H929" t="s">
         <v>4436</v>
       </c>
@@ -40432,6 +41406,9 @@
       <c r="C930">
         <v>421</v>
       </c>
+      <c r="G930" t="s">
+        <v>443</v>
+      </c>
       <c r="H930" t="s">
         <v>4439</v>
       </c>
@@ -40458,6 +41435,9 @@
       <c r="C931">
         <v>422</v>
       </c>
+      <c r="G931" t="s">
+        <v>443</v>
+      </c>
       <c r="H931" t="s">
         <v>4442</v>
       </c>
@@ -40484,6 +41464,9 @@
       <c r="C932">
         <v>423</v>
       </c>
+      <c r="G932" t="s">
+        <v>443</v>
+      </c>
       <c r="H932" t="s">
         <v>4445</v>
       </c>
@@ -40510,6 +41493,9 @@
       <c r="C933">
         <v>424</v>
       </c>
+      <c r="G933" t="s">
+        <v>443</v>
+      </c>
       <c r="H933" t="s">
         <v>4448</v>
       </c>
@@ -40536,6 +41522,9 @@
       <c r="C934">
         <v>13</v>
       </c>
+      <c r="G934" t="s">
+        <v>525</v>
+      </c>
       <c r="H934" t="s">
         <v>1892</v>
       </c>
@@ -40562,6 +41551,9 @@
       <c r="C935">
         <v>31</v>
       </c>
+      <c r="G935" t="s">
+        <v>1896</v>
+      </c>
       <c r="H935" t="s">
         <v>1896</v>
       </c>
@@ -40588,6 +41580,9 @@
       <c r="C936">
         <v>36</v>
       </c>
+      <c r="G936" t="s">
+        <v>525</v>
+      </c>
       <c r="H936" t="s">
         <v>1899</v>
       </c>
@@ -40614,6 +41609,9 @@
       <c r="C937">
         <v>91</v>
       </c>
+      <c r="G937" t="s">
+        <v>1902</v>
+      </c>
       <c r="H937" t="s">
         <v>1902</v>
       </c>
@@ -40640,6 +41638,9 @@
       <c r="C938">
         <v>94</v>
       </c>
+      <c r="G938" t="s">
+        <v>1905</v>
+      </c>
       <c r="H938" t="s">
         <v>1905</v>
       </c>
@@ -40666,6 +41667,9 @@
       <c r="C939">
         <v>101</v>
       </c>
+      <c r="G939" t="s">
+        <v>1908</v>
+      </c>
       <c r="H939" t="s">
         <v>1908</v>
       </c>
@@ -40692,6 +41696,9 @@
       <c r="C940">
         <v>113</v>
       </c>
+      <c r="G940" t="s">
+        <v>1911</v>
+      </c>
       <c r="H940" t="s">
         <v>1911</v>
       </c>
@@ -40718,6 +41725,9 @@
       <c r="C941">
         <v>119</v>
       </c>
+      <c r="G941" t="s">
+        <v>1914</v>
+      </c>
       <c r="H941" t="s">
         <v>1914</v>
       </c>
@@ -40744,6 +41754,9 @@
       <c r="C942">
         <v>134</v>
       </c>
+      <c r="G942" t="s">
+        <v>525</v>
+      </c>
       <c r="H942" t="s">
         <v>1917</v>
       </c>
@@ -40770,6 +41783,9 @@
       <c r="C943">
         <v>144</v>
       </c>
+      <c r="G943" t="s">
+        <v>1920</v>
+      </c>
       <c r="H943" t="s">
         <v>1920</v>
       </c>
@@ -40796,6 +41812,9 @@
       <c r="C944">
         <v>173</v>
       </c>
+      <c r="G944" t="s">
+        <v>1923</v>
+      </c>
       <c r="H944" t="s">
         <v>1923</v>
       </c>
@@ -40822,6 +41841,9 @@
       <c r="C945">
         <v>177</v>
       </c>
+      <c r="G945" t="s">
+        <v>525</v>
+      </c>
       <c r="H945" t="s">
         <v>1926</v>
       </c>
@@ -40848,6 +41870,9 @@
       <c r="C946">
         <v>211</v>
       </c>
+      <c r="G946" t="s">
+        <v>525</v>
+      </c>
       <c r="H946" t="s">
         <v>1929</v>
       </c>
@@ -40874,6 +41899,9 @@
       <c r="C947">
         <v>215</v>
       </c>
+      <c r="G947" t="s">
+        <v>525</v>
+      </c>
       <c r="H947" t="s">
         <v>1932</v>
       </c>
@@ -40900,6 +41928,9 @@
       <c r="C948">
         <v>250</v>
       </c>
+      <c r="G948" t="s">
+        <v>1935</v>
+      </c>
       <c r="H948" t="s">
         <v>1935</v>
       </c>
@@ -40926,6 +41957,9 @@
       <c r="C949">
         <v>284</v>
       </c>
+      <c r="G949" t="s">
+        <v>4666</v>
+      </c>
       <c r="H949" t="s">
         <v>1938</v>
       </c>
@@ -40952,6 +41986,9 @@
       <c r="C950">
         <v>291</v>
       </c>
+      <c r="G950" t="s">
+        <v>525</v>
+      </c>
       <c r="H950" t="s">
         <v>1940</v>
       </c>
@@ -40978,6 +42015,9 @@
       <c r="C951">
         <v>292</v>
       </c>
+      <c r="G951" t="s">
+        <v>1943</v>
+      </c>
       <c r="H951" t="s">
         <v>1943</v>
       </c>
@@ -41004,6 +42044,9 @@
       <c r="C952">
         <v>314</v>
       </c>
+      <c r="G952" t="s">
+        <v>1946</v>
+      </c>
       <c r="H952" t="s">
         <v>1946</v>
       </c>
@@ -41030,6 +42073,9 @@
       <c r="C953">
         <v>335</v>
       </c>
+      <c r="G953" t="s">
+        <v>525</v>
+      </c>
       <c r="H953" t="s">
         <v>1949</v>
       </c>
@@ -41056,6 +42102,9 @@
       <c r="C954">
         <v>337</v>
       </c>
+      <c r="G954" t="s">
+        <v>443</v>
+      </c>
       <c r="H954" t="s">
         <v>1952</v>
       </c>
@@ -41082,6 +42131,9 @@
       <c r="C955">
         <v>357</v>
       </c>
+      <c r="G955" t="s">
+        <v>4667</v>
+      </c>
       <c r="H955" t="s">
         <v>1955</v>
       </c>
@@ -41108,6 +42160,9 @@
       <c r="C956">
         <v>361</v>
       </c>
+      <c r="G956" t="s">
+        <v>4669</v>
+      </c>
       <c r="H956" t="s">
         <v>1958</v>
       </c>
@@ -41134,6 +42189,9 @@
       <c r="C957">
         <v>659</v>
       </c>
+      <c r="G957" t="s">
+        <v>4668</v>
+      </c>
       <c r="H957" t="s">
         <v>1961</v>
       </c>
@@ -41160,6 +42218,9 @@
       <c r="C958">
         <v>692</v>
       </c>
+      <c r="G958" t="s">
+        <v>4670</v>
+      </c>
       <c r="H958" t="s">
         <v>1964</v>
       </c>
@@ -41183,6 +42244,9 @@
       <c r="C959">
         <v>702</v>
       </c>
+      <c r="G959" t="s">
+        <v>4671</v>
+      </c>
       <c r="H959" t="s">
         <v>1966</v>
       </c>
@@ -41209,6 +42273,9 @@
       <c r="C960">
         <v>710</v>
       </c>
+      <c r="G960" t="s">
+        <v>4672</v>
+      </c>
       <c r="H960" t="s">
         <v>1969</v>
       </c>
@@ -41235,6 +42302,9 @@
       <c r="C961">
         <v>1084</v>
       </c>
+      <c r="G961" t="s">
+        <v>4673</v>
+      </c>
       <c r="H961" t="s">
         <v>1972</v>
       </c>
@@ -41261,6 +42331,9 @@
       <c r="C962">
         <v>1089</v>
       </c>
+      <c r="G962" t="s">
+        <v>4674</v>
+      </c>
       <c r="H962" t="s">
         <v>1975</v>
       </c>
@@ -41287,6 +42360,9 @@
       <c r="C963">
         <v>1099</v>
       </c>
+      <c r="G963" t="s">
+        <v>4675</v>
+      </c>
       <c r="H963" t="s">
         <v>1978</v>
       </c>
@@ -41313,6 +42389,9 @@
       <c r="C964">
         <v>1130</v>
       </c>
+      <c r="G964" t="s">
+        <v>4676</v>
+      </c>
       <c r="H964" t="s">
         <v>1981</v>
       </c>
@@ -41339,6 +42418,9 @@
       <c r="C965">
         <v>1132</v>
       </c>
+      <c r="G965" t="s">
+        <v>525</v>
+      </c>
       <c r="H965" t="s">
         <v>1983</v>
       </c>
@@ -41365,6 +42447,9 @@
       <c r="C966">
         <v>1133</v>
       </c>
+      <c r="G966" t="s">
+        <v>4677</v>
+      </c>
       <c r="H966" t="s">
         <v>1986</v>
       </c>
@@ -41391,6 +42476,9 @@
       <c r="C967">
         <v>1135</v>
       </c>
+      <c r="G967" t="s">
+        <v>4678</v>
+      </c>
       <c r="H967" t="s">
         <v>1989</v>
       </c>
@@ -41417,6 +42505,9 @@
       <c r="C968">
         <v>1168</v>
       </c>
+      <c r="G968" t="s">
+        <v>4679</v>
+      </c>
       <c r="H968" t="s">
         <v>1992</v>
       </c>
@@ -41443,6 +42534,9 @@
       <c r="C969">
         <v>1178</v>
       </c>
+      <c r="G969" t="s">
+        <v>443</v>
+      </c>
       <c r="H969" t="s">
         <v>1995</v>
       </c>
@@ -41469,6 +42563,9 @@
       <c r="C970">
         <v>1180</v>
       </c>
+      <c r="G970" t="s">
+        <v>4680</v>
+      </c>
       <c r="H970" t="s">
         <v>1998</v>
       </c>
@@ -41495,6 +42592,9 @@
       <c r="C971">
         <v>1181</v>
       </c>
+      <c r="G971" t="s">
+        <v>525</v>
+      </c>
       <c r="H971" t="s">
         <v>2001</v>
       </c>
@@ -41521,6 +42621,9 @@
       <c r="C972">
         <v>1182</v>
       </c>
+      <c r="G972" t="s">
+        <v>443</v>
+      </c>
       <c r="H972" t="s">
         <v>2004</v>
       </c>
@@ -41547,6 +42650,9 @@
       <c r="C973">
         <v>1189</v>
       </c>
+      <c r="G973" t="s">
+        <v>4681</v>
+      </c>
       <c r="H973" t="s">
         <v>2007</v>
       </c>
@@ -41573,6 +42679,9 @@
       <c r="C974">
         <v>1190</v>
       </c>
+      <c r="G974" t="s">
+        <v>4683</v>
+      </c>
       <c r="H974" t="s">
         <v>2010</v>
       </c>
@@ -41599,6 +42708,9 @@
       <c r="C975">
         <v>1191</v>
       </c>
+      <c r="G975" t="s">
+        <v>4684</v>
+      </c>
       <c r="H975" t="s">
         <v>2013</v>
       </c>
@@ -41625,6 +42737,9 @@
       <c r="C976">
         <v>1192</v>
       </c>
+      <c r="G976" t="s">
+        <v>4685</v>
+      </c>
       <c r="H976" t="s">
         <v>2016</v>
       </c>
@@ -41651,6 +42766,9 @@
       <c r="C977">
         <v>1193</v>
       </c>
+      <c r="G977" t="s">
+        <v>4682</v>
+      </c>
       <c r="H977" t="s">
         <v>2019</v>
       </c>
@@ -41677,6 +42795,9 @@
       <c r="C978">
         <v>1194</v>
       </c>
+      <c r="G978" t="s">
+        <v>4686</v>
+      </c>
       <c r="H978" t="s">
         <v>2022</v>
       </c>
@@ -41703,6 +42824,9 @@
       <c r="C979">
         <v>1195</v>
       </c>
+      <c r="G979" t="s">
+        <v>4687</v>
+      </c>
       <c r="H979" t="s">
         <v>2025</v>
       </c>
@@ -41729,6 +42853,9 @@
       <c r="C980">
         <v>1196</v>
       </c>
+      <c r="G980" t="s">
+        <v>443</v>
+      </c>
       <c r="H980" t="s">
         <v>2028</v>
       </c>
@@ -41755,6 +42882,9 @@
       <c r="C981">
         <v>1216</v>
       </c>
+      <c r="G981" t="s">
+        <v>525</v>
+      </c>
       <c r="H981" t="s">
         <v>2031</v>
       </c>
@@ -41781,6 +42911,9 @@
       <c r="C982">
         <v>1222</v>
       </c>
+      <c r="G982" t="s">
+        <v>4688</v>
+      </c>
       <c r="H982" t="s">
         <v>2033</v>
       </c>
@@ -41807,6 +42940,9 @@
       <c r="C983">
         <v>1233</v>
       </c>
+      <c r="G983" t="s">
+        <v>4689</v>
+      </c>
       <c r="H983" t="s">
         <v>2036</v>
       </c>
@@ -41833,6 +42969,9 @@
       <c r="C984">
         <v>1237</v>
       </c>
+      <c r="G984" t="s">
+        <v>443</v>
+      </c>
       <c r="H984" t="s">
         <v>2039</v>
       </c>
@@ -41859,6 +42998,9 @@
       <c r="C985">
         <v>1248</v>
       </c>
+      <c r="G985" t="s">
+        <v>4690</v>
+      </c>
       <c r="H985" t="s">
         <v>2042</v>
       </c>
@@ -41885,6 +43027,9 @@
       <c r="C986">
         <v>1256</v>
       </c>
+      <c r="G986" t="s">
+        <v>443</v>
+      </c>
       <c r="H986" t="s">
         <v>2045</v>
       </c>
@@ -41911,6 +43056,9 @@
       <c r="C987">
         <v>1263</v>
       </c>
+      <c r="G987" t="s">
+        <v>443</v>
+      </c>
       <c r="H987" t="s">
         <v>2048</v>
       </c>
@@ -41937,6 +43085,9 @@
       <c r="C988">
         <v>1264</v>
       </c>
+      <c r="G988" t="s">
+        <v>443</v>
+      </c>
       <c r="H988" t="s">
         <v>2051</v>
       </c>
@@ -41963,6 +43114,9 @@
       <c r="C989">
         <v>1265</v>
       </c>
+      <c r="G989" t="s">
+        <v>443</v>
+      </c>
       <c r="H989" t="s">
         <v>2054</v>
       </c>
@@ -41989,6 +43143,9 @@
       <c r="C990">
         <v>1266</v>
       </c>
+      <c r="G990" t="s">
+        <v>443</v>
+      </c>
       <c r="H990" t="s">
         <v>2057</v>
       </c>
@@ -42015,6 +43172,9 @@
       <c r="C991">
         <v>1289</v>
       </c>
+      <c r="G991" t="s">
+        <v>4691</v>
+      </c>
       <c r="H991" t="s">
         <v>2060</v>
       </c>
@@ -42041,6 +43201,9 @@
       <c r="C992">
         <v>1329</v>
       </c>
+      <c r="G992" t="s">
+        <v>4692</v>
+      </c>
       <c r="H992" t="s">
         <v>2063</v>
       </c>
@@ -42067,6 +43230,9 @@
       <c r="C993">
         <v>1332</v>
       </c>
+      <c r="G993" t="s">
+        <v>4693</v>
+      </c>
       <c r="H993" t="s">
         <v>2066</v>
       </c>
@@ -42093,6 +43259,9 @@
       <c r="C994">
         <v>1337</v>
       </c>
+      <c r="G994" t="s">
+        <v>4694</v>
+      </c>
       <c r="H994" t="s">
         <v>2068</v>
       </c>
@@ -42119,6 +43288,9 @@
       <c r="C995">
         <v>1338</v>
       </c>
+      <c r="G995" t="s">
+        <v>4695</v>
+      </c>
       <c r="H995" t="s">
         <v>2071</v>
       </c>
@@ -42145,6 +43317,9 @@
       <c r="C996">
         <v>1397</v>
       </c>
+      <c r="G996" t="s">
+        <v>4696</v>
+      </c>
       <c r="H996" t="s">
         <v>2074</v>
       </c>
@@ -42171,6 +43346,9 @@
       <c r="C997">
         <v>1402</v>
       </c>
+      <c r="G997" t="s">
+        <v>443</v>
+      </c>
       <c r="H997" t="s">
         <v>2076</v>
       </c>
@@ -42197,6 +43375,9 @@
       <c r="C998">
         <v>1435</v>
       </c>
+      <c r="G998" t="s">
+        <v>4697</v>
+      </c>
       <c r="H998" t="s">
         <v>2078</v>
       </c>
@@ -42223,6 +43404,9 @@
       <c r="C999">
         <v>1436</v>
       </c>
+      <c r="G999" t="s">
+        <v>4698</v>
+      </c>
       <c r="H999" t="s">
         <v>2080</v>
       </c>
@@ -42249,6 +43433,9 @@
       <c r="C1000">
         <v>1443</v>
       </c>
+      <c r="G1000" t="s">
+        <v>4699</v>
+      </c>
       <c r="H1000" t="s">
         <v>2082</v>
       </c>
@@ -42275,6 +43462,9 @@
       <c r="C1001">
         <v>1494</v>
       </c>
+      <c r="G1001" t="s">
+        <v>525</v>
+      </c>
       <c r="H1001" t="s">
         <v>2084</v>
       </c>
@@ -42301,6 +43491,9 @@
       <c r="C1002">
         <v>1648</v>
       </c>
+      <c r="G1002" t="s">
+        <v>525</v>
+      </c>
       <c r="H1002" t="s">
         <v>2086</v>
       </c>
@@ -42327,6 +43520,9 @@
       <c r="C1003">
         <v>1673</v>
       </c>
+      <c r="G1003" t="s">
+        <v>4700</v>
+      </c>
       <c r="H1003" t="s">
         <v>2089</v>
       </c>
@@ -42353,6 +43549,9 @@
       <c r="C1004">
         <v>1674</v>
       </c>
+      <c r="G1004" t="s">
+        <v>4701</v>
+      </c>
       <c r="H1004" t="s">
         <v>2092</v>
       </c>
@@ -42379,6 +43578,9 @@
       <c r="C1005">
         <v>1685</v>
       </c>
+      <c r="G1005" t="s">
+        <v>525</v>
+      </c>
       <c r="H1005" t="s">
         <v>2095</v>
       </c>
@@ -42405,6 +43607,9 @@
       <c r="C1006">
         <v>1688</v>
       </c>
+      <c r="G1006" t="s">
+        <v>4702</v>
+      </c>
       <c r="H1006" t="s">
         <v>2098</v>
       </c>
@@ -42431,6 +43636,9 @@
       <c r="C1007">
         <v>1704</v>
       </c>
+      <c r="G1007" t="s">
+        <v>4703</v>
+      </c>
       <c r="H1007" t="s">
         <v>2101</v>
       </c>
@@ -42457,6 +43665,9 @@
       <c r="C1008">
         <v>1718</v>
       </c>
+      <c r="G1008" t="s">
+        <v>443</v>
+      </c>
       <c r="H1008" t="s">
         <v>2103</v>
       </c>
@@ -42482,6 +43693,9 @@
       </c>
       <c r="C1009">
         <v>1721</v>
+      </c>
+      <c r="G1009" t="s">
+        <v>2107</v>
       </c>
       <c r="H1009" t="s">
         <v>2106</v>
@@ -42509,6 +43723,9 @@
       <c r="C1010">
         <v>16</v>
       </c>
+      <c r="G1010" t="s">
+        <v>4704</v>
+      </c>
       <c r="H1010" t="s">
         <v>3308</v>
       </c>
@@ -42535,6 +43752,9 @@
       <c r="C1011">
         <v>63</v>
       </c>
+      <c r="G1011" t="s">
+        <v>4712</v>
+      </c>
       <c r="H1011" t="s">
         <v>3441</v>
       </c>
@@ -42561,6 +43781,9 @@
       <c r="C1012">
         <v>98</v>
       </c>
+      <c r="G1012" t="s">
+        <v>443</v>
+      </c>
       <c r="H1012" t="s">
         <v>3536</v>
       </c>
@@ -42587,6 +43810,9 @@
       <c r="C1013">
         <v>101</v>
       </c>
+      <c r="G1013" t="s">
+        <v>525</v>
+      </c>
       <c r="H1013" t="s">
         <v>3545</v>
       </c>
@@ -42613,6 +43839,9 @@
       <c r="C1014">
         <v>163</v>
       </c>
+      <c r="G1014" t="s">
+        <v>443</v>
+      </c>
       <c r="H1014" t="s">
         <v>3725</v>
       </c>
@@ -42639,6 +43868,9 @@
       <c r="C1015">
         <v>235</v>
       </c>
+      <c r="G1015" t="s">
+        <v>525</v>
+      </c>
       <c r="H1015" t="s">
         <v>3939</v>
       </c>
@@ -42665,6 +43897,9 @@
       <c r="C1016">
         <v>251</v>
       </c>
+      <c r="G1016" t="s">
+        <v>525</v>
+      </c>
       <c r="H1016" t="s">
         <v>60</v>
       </c>
@@ -42691,6 +43926,9 @@
       <c r="C1017">
         <v>252</v>
       </c>
+      <c r="G1017" t="s">
+        <v>525</v>
+      </c>
       <c r="H1017" t="s">
         <v>3987</v>
       </c>
@@ -42717,6 +43955,9 @@
       <c r="C1018">
         <v>253</v>
       </c>
+      <c r="G1018" s="7" t="s">
+        <v>4713</v>
+      </c>
       <c r="H1018" t="s">
         <v>3990</v>
       </c>
@@ -42743,6 +43984,9 @@
       <c r="C1019">
         <v>290</v>
       </c>
+      <c r="G1019" t="s">
+        <v>4714</v>
+      </c>
       <c r="H1019" t="s">
         <v>4098</v>
       </c>
@@ -42769,6 +44013,9 @@
       <c r="C1020">
         <v>291</v>
       </c>
+      <c r="G1020" t="s">
+        <v>4715</v>
+      </c>
       <c r="H1020" t="s">
         <v>4101</v>
       </c>
@@ -42794,6 +44041,9 @@
       </c>
       <c r="C1021">
         <v>161</v>
+      </c>
+      <c r="G1021" t="s">
+        <v>4705</v>
       </c>
       <c r="H1021" t="s">
         <v>2109</v>
@@ -42821,6 +44071,9 @@
       <c r="C1022">
         <v>18</v>
       </c>
+      <c r="G1022" t="s">
+        <v>4716</v>
+      </c>
       <c r="H1022" t="s">
         <v>3314</v>
       </c>
@@ -42847,6 +44100,9 @@
       <c r="C1023">
         <v>19</v>
       </c>
+      <c r="G1023" t="s">
+        <v>4706</v>
+      </c>
       <c r="H1023" t="s">
         <v>3317</v>
       </c>
@@ -42873,6 +44129,9 @@
       <c r="C1024">
         <v>22</v>
       </c>
+      <c r="G1024" t="s">
+        <v>4707</v>
+      </c>
       <c r="H1024" t="s">
         <v>3325</v>
       </c>
@@ -42899,6 +44158,9 @@
       <c r="C1025">
         <v>41</v>
       </c>
+      <c r="G1025" s="7" t="s">
+        <v>4708</v>
+      </c>
       <c r="H1025" t="s">
         <v>3375</v>
       </c>
@@ -42925,6 +44187,9 @@
       <c r="C1026">
         <v>64</v>
       </c>
+      <c r="G1026" t="s">
+        <v>443</v>
+      </c>
       <c r="H1026" t="s">
         <v>3444</v>
       </c>
@@ -42951,6 +44216,9 @@
       <c r="C1027">
         <v>80</v>
       </c>
+      <c r="G1027" t="s">
+        <v>443</v>
+      </c>
       <c r="H1027" t="s">
         <v>3488</v>
       </c>
@@ -42977,6 +44245,9 @@
       <c r="C1028">
         <v>297</v>
       </c>
+      <c r="G1028" t="s">
+        <v>4717</v>
+      </c>
       <c r="H1028" t="s">
         <v>4119</v>
       </c>
@@ -43003,6 +44274,9 @@
       <c r="C1029">
         <v>300</v>
       </c>
+      <c r="G1029" t="s">
+        <v>443</v>
+      </c>
       <c r="H1029" t="s">
         <v>4128</v>
       </c>
@@ -43029,6 +44303,9 @@
       <c r="C1030">
         <v>357</v>
       </c>
+      <c r="G1030" t="s">
+        <v>525</v>
+      </c>
       <c r="H1030" t="s">
         <v>4269</v>
       </c>
@@ -43055,6 +44332,9 @@
       <c r="C1031">
         <v>358</v>
       </c>
+      <c r="G1031" t="s">
+        <v>525</v>
+      </c>
       <c r="H1031" t="s">
         <v>4272</v>
       </c>
@@ -43081,6 +44361,9 @@
       <c r="C1032">
         <v>364</v>
       </c>
+      <c r="G1032" t="s">
+        <v>443</v>
+      </c>
       <c r="H1032" t="s">
         <v>4286</v>
       </c>
@@ -43107,6 +44390,9 @@
       <c r="C1033">
         <v>378</v>
       </c>
+      <c r="G1033" t="s">
+        <v>443</v>
+      </c>
       <c r="H1033" t="s">
         <v>4323</v>
       </c>
@@ -43133,6 +44419,9 @@
       <c r="C1034">
         <v>379</v>
       </c>
+      <c r="G1034" t="s">
+        <v>443</v>
+      </c>
       <c r="H1034" t="s">
         <v>4325</v>
       </c>
@@ -43159,6 +44448,9 @@
       <c r="C1035">
         <v>384</v>
       </c>
+      <c r="G1035" t="s">
+        <v>443</v>
+      </c>
       <c r="H1035" t="s">
         <v>4339</v>
       </c>
@@ -43185,6 +44477,9 @@
       <c r="C1036">
         <v>386</v>
       </c>
+      <c r="G1036" t="s">
+        <v>443</v>
+      </c>
       <c r="H1036" t="s">
         <v>4344</v>
       </c>
@@ -43211,6 +44506,9 @@
       <c r="C1037">
         <v>387</v>
       </c>
+      <c r="G1037" t="s">
+        <v>443</v>
+      </c>
       <c r="H1037" t="s">
         <v>4346</v>
       </c>
@@ -43237,6 +44535,9 @@
       <c r="C1038">
         <v>390</v>
       </c>
+      <c r="G1038" t="s">
+        <v>443</v>
+      </c>
       <c r="H1038" t="s">
         <v>4354</v>
       </c>
@@ -43263,6 +44564,9 @@
       <c r="C1039">
         <v>391</v>
       </c>
+      <c r="G1039" t="s">
+        <v>443</v>
+      </c>
       <c r="H1039" t="s">
         <v>4356</v>
       </c>
@@ -43289,6 +44593,9 @@
       <c r="C1040">
         <v>402</v>
       </c>
+      <c r="G1040" t="s">
+        <v>443</v>
+      </c>
       <c r="H1040" t="s">
         <v>4385</v>
       </c>
@@ -43315,6 +44622,9 @@
       <c r="C1041">
         <v>403</v>
       </c>
+      <c r="G1041" t="s">
+        <v>4709</v>
+      </c>
       <c r="H1041" t="s">
         <v>4388</v>
       </c>
@@ -43341,6 +44651,9 @@
       <c r="C1042">
         <v>406</v>
       </c>
+      <c r="G1042" t="s">
+        <v>443</v>
+      </c>
       <c r="H1042" t="s">
         <v>4397</v>
       </c>
@@ -43367,6 +44680,9 @@
       <c r="C1043">
         <v>409</v>
       </c>
+      <c r="G1043" t="s">
+        <v>4405</v>
+      </c>
       <c r="H1043" t="s">
         <v>4405</v>
       </c>
@@ -43393,6 +44709,9 @@
       <c r="C1044">
         <v>413</v>
       </c>
+      <c r="G1044" t="s">
+        <v>4710</v>
+      </c>
       <c r="H1044" t="s">
         <v>4417</v>
       </c>
@@ -43419,6 +44738,9 @@
       <c r="C1045">
         <v>418</v>
       </c>
+      <c r="G1045" t="s">
+        <v>525</v>
+      </c>
       <c r="H1045" t="s">
         <v>4431</v>
       </c>
@@ -43445,6 +44767,9 @@
       <c r="C1046">
         <v>217</v>
       </c>
+      <c r="G1046" t="s">
+        <v>443</v>
+      </c>
       <c r="H1046" t="s">
         <v>3884</v>
       </c>
@@ -43471,6 +44796,9 @@
       <c r="C1047">
         <v>218</v>
       </c>
+      <c r="G1047" t="s">
+        <v>443</v>
+      </c>
       <c r="H1047" t="s">
         <v>3888</v>
       </c>
@@ -43497,6 +44825,9 @@
       <c r="C1048">
         <v>244</v>
       </c>
+      <c r="G1048" t="s">
+        <v>443</v>
+      </c>
       <c r="H1048" t="s">
         <v>2113</v>
       </c>
@@ -43523,6 +44854,9 @@
       <c r="C1049">
         <v>1556</v>
       </c>
+      <c r="G1049" t="s">
+        <v>443</v>
+      </c>
       <c r="H1049" t="s">
         <v>2117</v>
       </c>
@@ -43549,6 +44883,9 @@
       <c r="C1050">
         <v>1591</v>
       </c>
+      <c r="G1050" t="s">
+        <v>443</v>
+      </c>
       <c r="H1050" t="s">
         <v>2120</v>
       </c>
@@ -43574,6 +44911,9 @@
       </c>
       <c r="C1051">
         <v>1619</v>
+      </c>
+      <c r="G1051" t="s">
+        <v>443</v>
       </c>
       <c r="H1051" t="s">
         <v>2123</v>
@@ -43601,6 +44941,9 @@
       <c r="C1052">
         <v>106</v>
       </c>
+      <c r="G1052" t="s">
+        <v>443</v>
+      </c>
       <c r="H1052" t="s">
         <v>3558</v>
       </c>
@@ -43627,6 +44970,9 @@
       <c r="C1053">
         <v>109</v>
       </c>
+      <c r="G1053" t="s">
+        <v>443</v>
+      </c>
       <c r="H1053" t="s">
         <v>3567</v>
       </c>
@@ -43653,6 +44999,9 @@
       <c r="C1054">
         <v>142</v>
       </c>
+      <c r="G1054" t="s">
+        <v>443</v>
+      </c>
       <c r="H1054" t="s">
         <v>3661</v>
       </c>
@@ -43679,6 +45028,9 @@
       <c r="C1055">
         <v>171</v>
       </c>
+      <c r="G1055" t="s">
+        <v>443</v>
+      </c>
       <c r="H1055" t="s">
         <v>3749</v>
       </c>
@@ -43705,6 +45057,9 @@
       <c r="C1056">
         <v>489</v>
       </c>
+      <c r="G1056" t="s">
+        <v>4718</v>
+      </c>
       <c r="H1056" t="s">
         <v>2126</v>
       </c>
@@ -43730,6 +45085,9 @@
       </c>
       <c r="C1057">
         <v>663</v>
+      </c>
+      <c r="G1057" t="s">
+        <v>4719</v>
       </c>
       <c r="H1057" t="s">
         <v>2129</v>
@@ -43757,6 +45115,9 @@
       <c r="C1058">
         <v>5</v>
       </c>
+      <c r="G1058" s="7" t="s">
+        <v>4720</v>
+      </c>
       <c r="H1058" t="s">
         <v>3277</v>
       </c>
@@ -43783,6 +45144,9 @@
       <c r="C1059">
         <v>8</v>
       </c>
+      <c r="G1059" t="s">
+        <v>4721</v>
+      </c>
       <c r="H1059" t="s">
         <v>3286</v>
       </c>
@@ -43809,6 +45173,9 @@
       <c r="C1060">
         <v>14</v>
       </c>
+      <c r="G1060" t="s">
+        <v>525</v>
+      </c>
       <c r="H1060" t="s">
         <v>3303</v>
       </c>
@@ -43835,6 +45202,9 @@
       <c r="C1061">
         <v>29</v>
       </c>
+      <c r="G1061" t="s">
+        <v>525</v>
+      </c>
       <c r="H1061" t="s">
         <v>2142</v>
       </c>
@@ -43861,6 +45231,9 @@
       <c r="C1062">
         <v>52</v>
       </c>
+      <c r="G1062" t="s">
+        <v>525</v>
+      </c>
       <c r="H1062" t="s">
         <v>3408</v>
       </c>
@@ -43887,6 +45260,9 @@
       <c r="C1063">
         <v>53</v>
       </c>
+      <c r="G1063" t="s">
+        <v>525</v>
+      </c>
       <c r="H1063" t="s">
         <v>3411</v>
       </c>
@@ -43913,6 +45289,9 @@
       <c r="C1064">
         <v>99</v>
       </c>
+      <c r="G1064" t="s">
+        <v>4722</v>
+      </c>
       <c r="H1064" t="s">
         <v>3539</v>
       </c>
@@ -43939,6 +45318,9 @@
       <c r="C1065">
         <v>100</v>
       </c>
+      <c r="G1065" t="s">
+        <v>525</v>
+      </c>
       <c r="H1065" t="s">
         <v>3542</v>
       </c>
@@ -43965,6 +45347,9 @@
       <c r="C1066">
         <v>287</v>
       </c>
+      <c r="G1066" t="s">
+        <v>4723</v>
+      </c>
       <c r="H1066" t="s">
         <v>4089</v>
       </c>
@@ -43991,6 +45376,9 @@
       <c r="C1067">
         <v>7</v>
       </c>
+      <c r="G1067" t="s">
+        <v>4724</v>
+      </c>
       <c r="H1067" t="s">
         <v>2132</v>
       </c>
@@ -44017,6 +45405,9 @@
       <c r="C1068">
         <v>12</v>
       </c>
+      <c r="G1068" t="s">
+        <v>4725</v>
+      </c>
       <c r="H1068" t="s">
         <v>2135</v>
       </c>
@@ -44043,6 +45434,9 @@
       <c r="C1069">
         <v>21</v>
       </c>
+      <c r="G1069" t="s">
+        <v>525</v>
+      </c>
       <c r="H1069" t="s">
         <v>2138</v>
       </c>
@@ -44069,6 +45463,9 @@
       <c r="C1070">
         <v>152</v>
       </c>
+      <c r="G1070" t="s">
+        <v>4726</v>
+      </c>
       <c r="H1070" t="s">
         <v>2140</v>
       </c>
@@ -44095,6 +45492,9 @@
       <c r="C1071">
         <v>167</v>
       </c>
+      <c r="G1071" t="s">
+        <v>525</v>
+      </c>
       <c r="H1071" t="s">
         <v>2142</v>
       </c>
@@ -44121,6 +45521,9 @@
       <c r="C1072">
         <v>192</v>
       </c>
+      <c r="G1072" t="s">
+        <v>4727</v>
+      </c>
       <c r="H1072" t="s">
         <v>2145</v>
       </c>
@@ -44147,6 +45550,9 @@
       <c r="C1073">
         <v>280</v>
       </c>
+      <c r="G1073" t="s">
+        <v>4728</v>
+      </c>
       <c r="H1073" t="s">
         <v>2148</v>
       </c>
@@ -44173,6 +45579,9 @@
       <c r="C1074">
         <v>293</v>
       </c>
+      <c r="G1074" t="s">
+        <v>525</v>
+      </c>
       <c r="H1074" t="s">
         <v>2151</v>
       </c>
@@ -44199,6 +45608,9 @@
       <c r="C1075">
         <v>340</v>
       </c>
+      <c r="G1075" t="s">
+        <v>4665</v>
+      </c>
       <c r="H1075" t="s">
         <v>2153</v>
       </c>
@@ -44225,6 +45637,9 @@
       <c r="C1076">
         <v>342</v>
       </c>
+      <c r="G1076" t="s">
+        <v>4729</v>
+      </c>
       <c r="H1076" t="s">
         <v>2156</v>
       </c>
@@ -44251,6 +45666,9 @@
       <c r="C1077">
         <v>588</v>
       </c>
+      <c r="G1077" t="s">
+        <v>443</v>
+      </c>
       <c r="H1077" t="s">
         <v>2158</v>
       </c>
@@ -44277,6 +45695,9 @@
       <c r="C1078">
         <v>593</v>
       </c>
+      <c r="G1078" t="s">
+        <v>4730</v>
+      </c>
       <c r="H1078" t="s">
         <v>2161</v>
       </c>
@@ -44303,6 +45724,9 @@
       <c r="C1079">
         <v>594</v>
       </c>
+      <c r="G1079" t="s">
+        <v>4731</v>
+      </c>
       <c r="H1079" t="s">
         <v>2164</v>
       </c>
@@ -44329,6 +45753,9 @@
       <c r="C1080">
         <v>595</v>
       </c>
+      <c r="G1080" t="s">
+        <v>4732</v>
+      </c>
       <c r="H1080" t="s">
         <v>2167</v>
       </c>
@@ -44355,6 +45782,9 @@
       <c r="C1081">
         <v>611</v>
       </c>
+      <c r="G1081" t="s">
+        <v>4733</v>
+      </c>
       <c r="H1081" t="s">
         <v>2170</v>
       </c>
@@ -44381,6 +45811,9 @@
       <c r="C1082">
         <v>612</v>
       </c>
+      <c r="G1082" t="s">
+        <v>4734</v>
+      </c>
       <c r="H1082" t="s">
         <v>2172</v>
       </c>
@@ -44407,6 +45840,9 @@
       <c r="C1083">
         <v>613</v>
       </c>
+      <c r="G1083" t="s">
+        <v>4735</v>
+      </c>
       <c r="H1083" t="s">
         <v>2174</v>
       </c>
@@ -44433,6 +45869,9 @@
       <c r="C1084">
         <v>622</v>
       </c>
+      <c r="G1084" t="s">
+        <v>525</v>
+      </c>
       <c r="H1084" t="s">
         <v>2176</v>
       </c>
@@ -44459,6 +45898,9 @@
       <c r="C1085">
         <v>623</v>
       </c>
+      <c r="G1085" t="s">
+        <v>4736</v>
+      </c>
       <c r="H1085" t="s">
         <v>2179</v>
       </c>
@@ -44485,6 +45927,9 @@
       <c r="C1086">
         <v>634</v>
       </c>
+      <c r="G1086" t="s">
+        <v>4737</v>
+      </c>
       <c r="H1086" t="s">
         <v>2182</v>
       </c>
@@ -44511,6 +45956,9 @@
       <c r="C1087">
         <v>635</v>
       </c>
+      <c r="G1087" t="s">
+        <v>4738</v>
+      </c>
       <c r="H1087" t="s">
         <v>2185</v>
       </c>
@@ -44537,6 +45985,9 @@
       <c r="C1088">
         <v>638</v>
       </c>
+      <c r="G1088" t="s">
+        <v>4739</v>
+      </c>
       <c r="H1088" t="s">
         <v>2188</v>
       </c>
@@ -44563,6 +46014,9 @@
       <c r="C1089">
         <v>669</v>
       </c>
+      <c r="G1089" t="s">
+        <v>4740</v>
+      </c>
       <c r="H1089" t="s">
         <v>2191</v>
       </c>
@@ -44589,6 +46043,9 @@
       <c r="C1090">
         <v>688</v>
       </c>
+      <c r="G1090" t="s">
+        <v>4741</v>
+      </c>
       <c r="H1090" t="s">
         <v>2194</v>
       </c>
@@ -44615,6 +46072,9 @@
       <c r="C1091">
         <v>698</v>
       </c>
+      <c r="G1091" t="s">
+        <v>4742</v>
+      </c>
       <c r="H1091" t="s">
         <v>2197</v>
       </c>
@@ -44641,6 +46101,9 @@
       <c r="C1092">
         <v>708</v>
       </c>
+      <c r="G1092" t="s">
+        <v>4743</v>
+      </c>
       <c r="H1092" t="s">
         <v>2200</v>
       </c>
@@ -44667,6 +46130,9 @@
       <c r="C1093">
         <v>716</v>
       </c>
+      <c r="G1093" t="s">
+        <v>4744</v>
+      </c>
       <c r="H1093" t="s">
         <v>2203</v>
       </c>
@@ -44690,6 +46156,9 @@
       <c r="C1094">
         <v>720</v>
       </c>
+      <c r="G1094" t="s">
+        <v>4745</v>
+      </c>
       <c r="H1094" t="s">
         <v>2205</v>
       </c>
@@ -44716,6 +46185,9 @@
       <c r="C1095">
         <v>721</v>
       </c>
+      <c r="G1095" t="s">
+        <v>4746</v>
+      </c>
       <c r="H1095" t="s">
         <v>2208</v>
       </c>
@@ -44742,6 +46214,9 @@
       <c r="C1096">
         <v>749</v>
       </c>
+      <c r="G1096" t="s">
+        <v>4747</v>
+      </c>
       <c r="H1096" t="s">
         <v>2210</v>
       </c>
@@ -44768,6 +46243,9 @@
       <c r="C1097">
         <v>863</v>
       </c>
+      <c r="G1097" t="s">
+        <v>2213</v>
+      </c>
       <c r="H1097" t="s">
         <v>2213</v>
       </c>
@@ -44794,6 +46272,9 @@
       <c r="C1098">
         <v>895</v>
       </c>
+      <c r="G1098" t="s">
+        <v>525</v>
+      </c>
       <c r="H1098" t="s">
         <v>2216</v>
       </c>
@@ -44820,6 +46301,9 @@
       <c r="C1099">
         <v>896</v>
       </c>
+      <c r="G1099" t="s">
+        <v>4748</v>
+      </c>
       <c r="H1099" t="s">
         <v>2218</v>
       </c>
@@ -44846,6 +46330,9 @@
       <c r="C1100">
         <v>897</v>
       </c>
+      <c r="G1100" t="s">
+        <v>443</v>
+      </c>
       <c r="H1100" t="s">
         <v>2220</v>
       </c>
@@ -44872,6 +46359,9 @@
       <c r="C1101">
         <v>916</v>
       </c>
+      <c r="G1101" t="s">
+        <v>2222</v>
+      </c>
       <c r="H1101" t="s">
         <v>2222</v>
       </c>
@@ -44898,6 +46388,9 @@
       <c r="C1102">
         <v>917</v>
       </c>
+      <c r="G1102" t="s">
+        <v>2225</v>
+      </c>
       <c r="H1102" t="s">
         <v>2225</v>
       </c>
@@ -44924,6 +46417,9 @@
       <c r="C1103">
         <v>918</v>
       </c>
+      <c r="G1103" t="s">
+        <v>525</v>
+      </c>
       <c r="H1103" t="s">
         <v>2228</v>
       </c>
@@ -44950,6 +46446,9 @@
       <c r="C1104">
         <v>919</v>
       </c>
+      <c r="G1104" t="s">
+        <v>525</v>
+      </c>
       <c r="H1104" t="s">
         <v>2231</v>
       </c>
@@ -44976,6 +46475,9 @@
       <c r="C1105">
         <v>920</v>
       </c>
+      <c r="G1105" t="s">
+        <v>2234</v>
+      </c>
       <c r="H1105" t="s">
         <v>2234</v>
       </c>
@@ -45002,6 +46504,9 @@
       <c r="C1106">
         <v>972</v>
       </c>
+      <c r="G1106" t="s">
+        <v>4749</v>
+      </c>
       <c r="H1106" t="s">
         <v>2237</v>
       </c>
@@ -45028,6 +46533,9 @@
       <c r="C1107">
         <v>1261</v>
       </c>
+      <c r="G1107" t="s">
+        <v>525</v>
+      </c>
       <c r="H1107" t="s">
         <v>2240</v>
       </c>
@@ -45054,6 +46562,9 @@
       <c r="C1108">
         <v>1547</v>
       </c>
+      <c r="G1108" t="s">
+        <v>4751</v>
+      </c>
       <c r="H1108" t="s">
         <v>2243</v>
       </c>
@@ -45080,6 +46591,9 @@
       <c r="C1109">
         <v>1629</v>
       </c>
+      <c r="G1109" t="s">
+        <v>4750</v>
+      </c>
       <c r="H1109" t="s">
         <v>2246</v>
       </c>
@@ -45106,6 +46620,9 @@
       <c r="C1110">
         <v>1714</v>
       </c>
+      <c r="G1110" t="s">
+        <v>525</v>
+      </c>
       <c r="H1110" t="s">
         <v>2248</v>
       </c>
@@ -45132,6 +46649,9 @@
       <c r="C1111">
         <v>1715</v>
       </c>
+      <c r="G1111" t="s">
+        <v>525</v>
+      </c>
       <c r="H1111" t="s">
         <v>2251</v>
       </c>
@@ -45157,6 +46677,9 @@
       </c>
       <c r="C1112">
         <v>1717</v>
+      </c>
+      <c r="G1112" t="s">
+        <v>443</v>
       </c>
       <c r="H1112" t="s">
         <v>2254</v>
@@ -45184,6 +46707,9 @@
       <c r="C1113">
         <v>404</v>
       </c>
+      <c r="G1113" t="s">
+        <v>4752</v>
+      </c>
       <c r="H1113" t="s">
         <v>4391</v>
       </c>
@@ -45210,6 +46736,9 @@
       <c r="C1114">
         <v>405</v>
       </c>
+      <c r="G1114" t="s">
+        <v>4753</v>
+      </c>
       <c r="H1114" t="s">
         <v>4394</v>
       </c>
@@ -45236,6 +46765,9 @@
       <c r="C1115">
         <v>56</v>
       </c>
+      <c r="G1115" t="s">
+        <v>4754</v>
+      </c>
       <c r="H1115" t="s">
         <v>2257</v>
       </c>
@@ -45262,6 +46794,9 @@
       <c r="C1116">
         <v>70</v>
       </c>
+      <c r="G1116" t="s">
+        <v>4755</v>
+      </c>
       <c r="H1116" t="s">
         <v>2261</v>
       </c>
@@ -45288,6 +46823,9 @@
       <c r="C1117">
         <v>103</v>
       </c>
+      <c r="G1117" t="s">
+        <v>4756</v>
+      </c>
       <c r="H1117" t="s">
         <v>2264</v>
       </c>
@@ -45314,6 +46852,9 @@
       <c r="C1118">
         <v>116</v>
       </c>
+      <c r="G1118" t="s">
+        <v>525</v>
+      </c>
       <c r="H1118" t="s">
         <v>2267</v>
       </c>
@@ -45340,6 +46881,9 @@
       <c r="C1119">
         <v>137</v>
       </c>
+      <c r="G1119" t="s">
+        <v>525</v>
+      </c>
       <c r="H1119" t="s">
         <v>2270</v>
       </c>
@@ -45366,6 +46910,9 @@
       <c r="C1120">
         <v>141</v>
       </c>
+      <c r="G1120" t="s">
+        <v>443</v>
+      </c>
       <c r="H1120" t="s">
         <v>2273</v>
       </c>
@@ -45392,6 +46939,9 @@
       <c r="C1121">
         <v>202</v>
       </c>
+      <c r="G1121" t="s">
+        <v>525</v>
+      </c>
       <c r="H1121" t="s">
         <v>2276</v>
       </c>
@@ -45418,6 +46968,9 @@
       <c r="C1122">
         <v>203</v>
       </c>
+      <c r="G1122" t="s">
+        <v>4757</v>
+      </c>
       <c r="H1122" t="s">
         <v>2279</v>
       </c>
@@ -45444,6 +46997,9 @@
       <c r="C1123">
         <v>257</v>
       </c>
+      <c r="G1123" t="s">
+        <v>4758</v>
+      </c>
       <c r="H1123" t="s">
         <v>2282</v>
       </c>
@@ -45470,6 +47026,9 @@
       <c r="C1124">
         <v>332</v>
       </c>
+      <c r="G1124" t="s">
+        <v>525</v>
+      </c>
       <c r="H1124" t="s">
         <v>2285</v>
       </c>
@@ -45496,6 +47055,9 @@
       <c r="C1125">
         <v>580</v>
       </c>
+      <c r="G1125" t="s">
+        <v>525</v>
+      </c>
       <c r="H1125" t="s">
         <v>2288</v>
       </c>
@@ -45522,6 +47084,9 @@
       <c r="C1126">
         <v>1028</v>
       </c>
+      <c r="G1126" t="s">
+        <v>4711</v>
+      </c>
       <c r="H1126" t="s">
         <v>2291</v>
       </c>
@@ -45548,6 +47113,9 @@
       <c r="C1127">
         <v>1158</v>
       </c>
+      <c r="G1127" t="s">
+        <v>443</v>
+      </c>
       <c r="H1127" t="s">
         <v>2294</v>
       </c>
@@ -45574,6 +47142,9 @@
       <c r="C1128">
         <v>1336</v>
       </c>
+      <c r="G1128" t="s">
+        <v>4759</v>
+      </c>
       <c r="H1128" t="s">
         <v>2297</v>
       </c>
@@ -45600,6 +47171,9 @@
       <c r="C1129">
         <v>1382</v>
       </c>
+      <c r="G1129" t="s">
+        <v>525</v>
+      </c>
       <c r="H1129" t="s">
         <v>2300</v>
       </c>
@@ -45626,6 +47200,9 @@
       <c r="C1130">
         <v>1421</v>
       </c>
+      <c r="G1130" t="s">
+        <v>4760</v>
+      </c>
       <c r="H1130" t="s">
         <v>2303</v>
       </c>
@@ -45652,6 +47229,9 @@
       <c r="C1131">
         <v>1422</v>
       </c>
+      <c r="G1131" t="s">
+        <v>525</v>
+      </c>
       <c r="H1131" t="s">
         <v>2306</v>
       </c>
@@ -45678,6 +47258,9 @@
       <c r="C1132">
         <v>1480</v>
       </c>
+      <c r="G1132" t="s">
+        <v>2308</v>
+      </c>
       <c r="H1132" t="s">
         <v>2308</v>
       </c>
@@ -45703,6 +47286,9 @@
       </c>
       <c r="C1133">
         <v>1699</v>
+      </c>
+      <c r="G1133" t="s">
+        <v>525</v>
       </c>
       <c r="H1133" t="s">
         <v>2310</v>
@@ -45730,6 +47316,9 @@
       <c r="C1134">
         <v>2</v>
       </c>
+      <c r="G1134" t="s">
+        <v>443</v>
+      </c>
       <c r="H1134" t="s">
         <v>3269</v>
       </c>
@@ -45756,6 +47345,9 @@
       <c r="C1135">
         <v>6</v>
       </c>
+      <c r="G1135" t="s">
+        <v>443</v>
+      </c>
       <c r="H1135" t="s">
         <v>3279</v>
       </c>
@@ -45782,6 +47374,9 @@
       <c r="C1136">
         <v>9</v>
       </c>
+      <c r="G1136" t="s">
+        <v>525</v>
+      </c>
       <c r="H1136" t="s">
         <v>3289</v>
       </c>
@@ -45808,6 +47403,9 @@
       <c r="C1137">
         <v>15</v>
       </c>
+      <c r="G1137" t="s">
+        <v>4761</v>
+      </c>
       <c r="H1137" t="s">
         <v>3305</v>
       </c>
@@ -45834,6 +47432,9 @@
       <c r="C1138">
         <v>17</v>
       </c>
+      <c r="G1138" t="s">
+        <v>4762</v>
+      </c>
       <c r="H1138" t="s">
         <v>3311</v>
       </c>
@@ -45860,6 +47461,9 @@
       <c r="C1139">
         <v>20</v>
       </c>
+      <c r="G1139" t="s">
+        <v>4763</v>
+      </c>
       <c r="H1139" t="s">
         <v>3320</v>
       </c>
@@ -45886,6 +47490,9 @@
       <c r="C1140">
         <v>28</v>
       </c>
+      <c r="G1140" t="s">
+        <v>4764</v>
+      </c>
       <c r="H1140" t="s">
         <v>3341</v>
       </c>
@@ -45912,6 +47519,9 @@
       <c r="C1141">
         <v>32</v>
       </c>
+      <c r="G1141" t="s">
+        <v>4765</v>
+      </c>
       <c r="H1141" t="s">
         <v>3352</v>
       </c>
@@ -45938,6 +47548,9 @@
       <c r="C1142">
         <v>43</v>
       </c>
+      <c r="G1142" t="s">
+        <v>443</v>
+      </c>
       <c r="H1142" t="s">
         <v>3379</v>
       </c>
@@ -45964,6 +47577,9 @@
       <c r="C1143">
         <v>49</v>
       </c>
+      <c r="G1143" t="s">
+        <v>525</v>
+      </c>
       <c r="H1143" t="s">
         <v>3397</v>
       </c>
@@ -45990,6 +47606,9 @@
       <c r="C1144">
         <v>54</v>
       </c>
+      <c r="G1144" t="s">
+        <v>4766</v>
+      </c>
       <c r="H1144" t="s">
         <v>3414</v>
       </c>
@@ -46016,6 +47635,9 @@
       <c r="C1145">
         <v>57</v>
       </c>
+      <c r="G1145" t="s">
+        <v>4767</v>
+      </c>
       <c r="H1145" t="s">
         <v>3424</v>
       </c>
@@ -46042,6 +47664,9 @@
       <c r="C1146">
         <v>61</v>
       </c>
+      <c r="G1146" t="s">
+        <v>4768</v>
+      </c>
       <c r="H1146" t="s">
         <v>3437</v>
       </c>
@@ -46068,6 +47693,9 @@
       <c r="C1147">
         <v>69</v>
       </c>
+      <c r="G1147" t="s">
+        <v>443</v>
+      </c>
       <c r="H1147" t="s">
         <v>3457</v>
       </c>
@@ -46094,6 +47722,9 @@
       <c r="C1148">
         <v>76</v>
       </c>
+      <c r="G1148" t="s">
+        <v>4769</v>
+      </c>
       <c r="H1148" t="s">
         <v>3476</v>
       </c>
@@ -46120,6 +47751,9 @@
       <c r="C1149">
         <v>79</v>
       </c>
+      <c r="G1149" t="s">
+        <v>4770</v>
+      </c>
       <c r="H1149" t="s">
         <v>3485</v>
       </c>
@@ -46146,6 +47780,9 @@
       <c r="C1150">
         <v>81</v>
       </c>
+      <c r="G1150" t="s">
+        <v>443</v>
+      </c>
       <c r="H1150" t="s">
         <v>3490</v>
       </c>
@@ -46172,6 +47809,9 @@
       <c r="C1151">
         <v>87</v>
       </c>
+      <c r="G1151" t="s">
+        <v>443</v>
+      </c>
       <c r="H1151" t="s">
         <v>3505</v>
       </c>
@@ -46198,6 +47838,9 @@
       <c r="C1152">
         <v>94</v>
       </c>
+      <c r="G1152" t="s">
+        <v>443</v>
+      </c>
       <c r="H1152" t="s">
         <v>3526</v>
       </c>
@@ -46224,6 +47867,9 @@
       <c r="C1153">
         <v>96</v>
       </c>
+      <c r="G1153" t="s">
+        <v>525</v>
+      </c>
       <c r="H1153" t="s">
         <v>3531</v>
       </c>
@@ -46250,6 +47896,9 @@
       <c r="C1154">
         <v>130</v>
       </c>
+      <c r="G1154" t="s">
+        <v>443</v>
+      </c>
       <c r="H1154" t="s">
         <v>3627</v>
       </c>
@@ -46276,6 +47925,9 @@
       <c r="C1155">
         <v>144</v>
       </c>
+      <c r="G1155" t="s">
+        <v>443</v>
+      </c>
       <c r="H1155" t="s">
         <v>3667</v>
       </c>
@@ -46302,6 +47954,9 @@
       <c r="C1156">
         <v>146</v>
       </c>
+      <c r="G1156" t="s">
+        <v>443</v>
+      </c>
       <c r="H1156" t="s">
         <v>3673</v>
       </c>
@@ -46328,6 +47983,9 @@
       <c r="C1157">
         <v>149</v>
       </c>
+      <c r="G1157" t="s">
+        <v>443</v>
+      </c>
       <c r="H1157" t="s">
         <v>3682</v>
       </c>
@@ -46354,6 +48012,9 @@
       <c r="C1158">
         <v>153</v>
       </c>
+      <c r="G1158" t="s">
+        <v>443</v>
+      </c>
       <c r="H1158" t="s">
         <v>3694</v>
       </c>
@@ -46380,6 +48041,9 @@
       <c r="C1159">
         <v>191</v>
       </c>
+      <c r="G1159" t="s">
+        <v>525</v>
+      </c>
       <c r="H1159" t="s">
         <v>1862</v>
       </c>
@@ -46406,6 +48070,9 @@
       <c r="C1160">
         <v>195</v>
       </c>
+      <c r="G1160" t="s">
+        <v>4771</v>
+      </c>
       <c r="H1160" t="s">
         <v>3820</v>
       </c>
@@ -46432,6 +48099,9 @@
       <c r="C1161">
         <v>200</v>
       </c>
+      <c r="G1161" t="s">
+        <v>4772</v>
+      </c>
       <c r="H1161" t="s">
         <v>3833</v>
       </c>
@@ -46458,6 +48128,9 @@
       <c r="C1162">
         <v>227</v>
       </c>
+      <c r="G1162" s="8" t="s">
+        <v>4773</v>
+      </c>
       <c r="H1162" t="s">
         <v>3916</v>
       </c>
@@ -46484,6 +48157,9 @@
       <c r="C1163">
         <v>231</v>
       </c>
+      <c r="G1163" s="7" t="s">
+        <v>4774</v>
+      </c>
       <c r="H1163" t="s">
         <v>3927</v>
       </c>
@@ -46510,6 +48186,9 @@
       <c r="C1164">
         <v>232</v>
       </c>
+      <c r="G1164" t="s">
+        <v>525</v>
+      </c>
       <c r="H1164" t="s">
         <v>3930</v>
       </c>
@@ -46536,6 +48215,9 @@
       <c r="C1165">
         <v>234</v>
       </c>
+      <c r="G1165" t="s">
+        <v>4775</v>
+      </c>
       <c r="H1165" t="s">
         <v>3936</v>
       </c>
@@ -46562,6 +48244,9 @@
       <c r="C1166">
         <v>237</v>
       </c>
+      <c r="G1166" t="s">
+        <v>525</v>
+      </c>
       <c r="H1166" t="s">
         <v>3945</v>
       </c>
@@ -46588,6 +48273,9 @@
       <c r="C1167">
         <v>242</v>
       </c>
+      <c r="G1167" t="s">
+        <v>525</v>
+      </c>
       <c r="H1167" t="s">
         <v>2261</v>
       </c>
@@ -46614,6 +48302,9 @@
       <c r="C1168">
         <v>244</v>
       </c>
+      <c r="G1168" s="7" t="s">
+        <v>4776</v>
+      </c>
       <c r="H1168" t="s">
         <v>3965</v>
       </c>
@@ -46640,6 +48331,9 @@
       <c r="C1169">
         <v>245</v>
       </c>
+      <c r="G1169" t="s">
+        <v>4777</v>
+      </c>
       <c r="H1169" t="s">
         <v>3968</v>
       </c>
@@ -46666,6 +48360,9 @@
       <c r="C1170">
         <v>246</v>
       </c>
+      <c r="G1170" t="s">
+        <v>4778</v>
+      </c>
       <c r="H1170" t="s">
         <v>3971</v>
       </c>
@@ -46692,6 +48389,9 @@
       <c r="C1171">
         <v>286</v>
       </c>
+      <c r="G1171" t="s">
+        <v>4779</v>
+      </c>
       <c r="H1171" t="s">
         <v>4086</v>
       </c>
@@ -46718,6 +48418,9 @@
       <c r="C1172">
         <v>288</v>
       </c>
+      <c r="G1172" t="s">
+        <v>525</v>
+      </c>
       <c r="H1172" t="s">
         <v>4092</v>
       </c>
@@ -46744,6 +48447,9 @@
       <c r="C1173">
         <v>289</v>
       </c>
+      <c r="G1173" t="s">
+        <v>525</v>
+      </c>
       <c r="H1173" t="s">
         <v>4095</v>
       </c>
@@ -46770,6 +48476,9 @@
       <c r="C1174">
         <v>292</v>
       </c>
+      <c r="G1174" t="s">
+        <v>4780</v>
+      </c>
       <c r="H1174" t="s">
         <v>4104</v>
       </c>
@@ -46796,6 +48505,9 @@
       <c r="C1175">
         <v>298</v>
       </c>
+      <c r="G1175" t="s">
+        <v>4781</v>
+      </c>
       <c r="H1175" t="s">
         <v>4122</v>
       </c>
@@ -46822,6 +48534,9 @@
       <c r="C1176">
         <v>299</v>
       </c>
+      <c r="G1176" t="s">
+        <v>4782</v>
+      </c>
       <c r="H1176" t="s">
         <v>4125</v>
       </c>
@@ -46848,6 +48563,9 @@
       <c r="C1177">
         <v>346</v>
       </c>
+      <c r="G1177" t="s">
+        <v>443</v>
+      </c>
       <c r="H1177" t="s">
         <v>4239</v>
       </c>
@@ -46874,6 +48592,9 @@
       <c r="C1178">
         <v>392</v>
       </c>
+      <c r="G1178" t="s">
+        <v>525</v>
+      </c>
       <c r="H1178" t="s">
         <v>1940</v>
       </c>
@@ -46900,6 +48621,9 @@
       <c r="C1179">
         <v>417</v>
       </c>
+      <c r="G1179" t="s">
+        <v>4783</v>
+      </c>
       <c r="H1179" t="s">
         <v>4428</v>
       </c>
@@ -46926,6 +48650,9 @@
       <c r="C1180">
         <v>225</v>
       </c>
+      <c r="G1180" t="s">
+        <v>525</v>
+      </c>
       <c r="H1180" t="s">
         <v>3909</v>
       </c>
@@ -46952,6 +48679,9 @@
       <c r="C1181">
         <v>226</v>
       </c>
+      <c r="G1181" t="s">
+        <v>525</v>
+      </c>
       <c r="H1181" t="s">
         <v>3913</v>
       </c>
@@ -46978,6 +48708,9 @@
       <c r="C1182">
         <v>243</v>
       </c>
+      <c r="G1182" t="s">
+        <v>443</v>
+      </c>
       <c r="H1182" t="s">
         <v>3961</v>
       </c>
@@ -47003,6 +48736,9 @@
       </c>
       <c r="C1183">
         <v>17</v>
+      </c>
+      <c r="G1183" t="s">
+        <v>443</v>
       </c>
       <c r="H1183" t="s">
         <v>2313</v>
@@ -47030,6 +48766,9 @@
       <c r="C1184">
         <v>89</v>
       </c>
+      <c r="G1184" t="s">
+        <v>443</v>
+      </c>
       <c r="H1184" t="s">
         <v>3511</v>
       </c>
@@ -47056,6 +48795,9 @@
       <c r="C1185">
         <v>90</v>
       </c>
+      <c r="G1185" t="s">
+        <v>443</v>
+      </c>
       <c r="H1185" t="s">
         <v>3514</v>
       </c>
@@ -47082,6 +48824,9 @@
       <c r="C1186">
         <v>92</v>
       </c>
+      <c r="G1186" t="s">
+        <v>443</v>
+      </c>
       <c r="H1186" t="s">
         <v>3520</v>
       </c>
@@ -47108,6 +48853,9 @@
       <c r="C1187">
         <v>93</v>
       </c>
+      <c r="G1187" t="s">
+        <v>443</v>
+      </c>
       <c r="H1187" t="s">
         <v>3523</v>
       </c>
@@ -47134,6 +48882,9 @@
       <c r="C1188">
         <v>143</v>
       </c>
+      <c r="G1188" t="s">
+        <v>443</v>
+      </c>
       <c r="H1188" t="s">
         <v>3664</v>
       </c>
@@ -47160,6 +48911,9 @@
       <c r="C1189">
         <v>145</v>
       </c>
+      <c r="G1189" t="s">
+        <v>443</v>
+      </c>
       <c r="H1189" t="s">
         <v>3670</v>
       </c>
@@ -47186,6 +48940,9 @@
       <c r="C1190">
         <v>147</v>
       </c>
+      <c r="G1190" t="s">
+        <v>443</v>
+      </c>
       <c r="H1190" t="s">
         <v>3676</v>
       </c>
@@ -47212,6 +48969,9 @@
       <c r="C1191">
         <v>162</v>
       </c>
+      <c r="G1191" t="s">
+        <v>443</v>
+      </c>
       <c r="H1191" t="s">
         <v>3722</v>
       </c>
@@ -47238,6 +48998,9 @@
       <c r="C1192">
         <v>199</v>
       </c>
+      <c r="G1192" t="s">
+        <v>443</v>
+      </c>
       <c r="H1192" t="s">
         <v>3830</v>
       </c>
@@ -47264,6 +49027,9 @@
       <c r="C1193">
         <v>216</v>
       </c>
+      <c r="G1193" t="s">
+        <v>443</v>
+      </c>
       <c r="H1193" t="s">
         <v>3881</v>
       </c>
@@ -47290,6 +49056,9 @@
       <c r="C1194">
         <v>230</v>
       </c>
+      <c r="G1194" t="s">
+        <v>525</v>
+      </c>
       <c r="H1194" t="s">
         <v>3925</v>
       </c>
@@ -47315,6 +49084,9 @@
       </c>
       <c r="C1195">
         <v>304</v>
+      </c>
+      <c r="G1195" t="s">
+        <v>443</v>
       </c>
       <c r="H1195" t="s">
         <v>4137</v>

</xml_diff>

<commit_message>
add new method classes
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
+++ b/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB4480D-F7F1-420A-8F83-EDEE46104C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6ABB1A-CBDE-4C56-BCEC-B765BA9AAD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
   </bookViews>
   <sheets>
     <sheet name="amber+cpptraj" sheetId="1" r:id="rId1"/>
@@ -15369,8 +15369,8 @@
   <dimension ref="A1:L1669"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1026" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1196" sqref="G1196"/>
+      <pane ySplit="1" topLeftCell="A1050" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1066" sqref="G1066"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44594,7 +44594,7 @@
         <v>402</v>
       </c>
       <c r="G1040" t="s">
-        <v>443</v>
+        <v>525</v>
       </c>
       <c r="H1040" t="s">
         <v>4385</v>

</xml_diff>

<commit_message>
import more terms from UO, add components, and generate full version
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
+++ b/src/ontology/terms-extraction/amber and cpptraj term addition status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84965688-FB0F-46BA-9F4C-E8168B290AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FB0AE5-3F36-4715-84B3-667E892274CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{6233D32F-FD8F-498C-A153-5C7121F5D6FF}"/>
   </bookViews>
@@ -585,12 +585,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1667" authorId="0" shapeId="0" xr:uid="{2178981D-AFD7-4156-B9B6-9C0BB1E75B34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+due to formatting problem, it is unclear what it actually refers to
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11991" uniqueCount="5077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12007" uniqueCount="5084">
   <si>
     <t>skip? (-=yes)</t>
   </si>
@@ -15821,13 +15846,34 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000062</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000325</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000221</t>
+  </si>
+  <si>
+    <t>elementary charge</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000324</t>
+  </si>
+  <si>
+    <t>debye</t>
+  </si>
+  <si>
+    <t>centimeter square per second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15903,6 +15949,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -15943,7 +15999,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -15960,6 +16016,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16277,9 +16335,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF52D84-4AB6-470B-8703-41185DC33D82}">
   <dimension ref="A1:L1669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1552" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1561" sqref="H1561"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1649" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1658" sqref="G1658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -65229,7 +65287,9 @@
       <c r="C1654">
         <v>26</v>
       </c>
-      <c r="G1654" s="8"/>
+      <c r="G1654" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="H1654" t="s">
         <v>3252</v>
       </c>
@@ -65256,7 +65316,9 @@
       <c r="C1655">
         <v>160</v>
       </c>
-      <c r="G1655" s="8"/>
+      <c r="G1655" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="H1655" t="s">
         <v>3256</v>
       </c>
@@ -65283,7 +65345,9 @@
       <c r="C1656">
         <v>1627</v>
       </c>
-      <c r="G1656" s="8"/>
+      <c r="G1656" s="8" t="s">
+        <v>524</v>
+      </c>
       <c r="H1656" t="s">
         <v>3258</v>
       </c>
@@ -65310,7 +65374,9 @@
       <c r="C1657">
         <v>1628</v>
       </c>
-      <c r="G1657" s="8"/>
+      <c r="G1657" s="15" t="s">
+        <v>5077</v>
+      </c>
       <c r="H1657" t="s">
         <v>3261</v>
       </c>
@@ -65337,7 +65403,9 @@
       <c r="C1658">
         <v>24</v>
       </c>
-      <c r="G1658" s="8"/>
+      <c r="G1658" s="14" t="s">
+        <v>524</v>
+      </c>
       <c r="H1658" t="s">
         <v>3256</v>
       </c>
@@ -65364,7 +65432,9 @@
       <c r="C1659">
         <v>47</v>
       </c>
-      <c r="G1659" s="8"/>
+      <c r="G1659" s="14" t="s">
+        <v>524</v>
+      </c>
       <c r="H1659" t="s">
         <v>3390</v>
       </c>
@@ -65391,7 +65461,9 @@
       <c r="C1660">
         <v>102</v>
       </c>
-      <c r="G1660" s="8"/>
+      <c r="G1660" s="14" t="s">
+        <v>442</v>
+      </c>
       <c r="H1660" t="s">
         <v>3547</v>
       </c>
@@ -65418,7 +65490,9 @@
       <c r="C1661">
         <v>103</v>
       </c>
-      <c r="G1661" s="8"/>
+      <c r="G1661" s="14" t="s">
+        <v>524</v>
+      </c>
       <c r="H1661" t="s">
         <v>3252</v>
       </c>
@@ -65445,7 +65519,9 @@
       <c r="C1662">
         <v>104</v>
       </c>
-      <c r="G1662" s="8"/>
+      <c r="G1662" s="14" t="s">
+        <v>5079</v>
+      </c>
       <c r="H1662" t="s">
         <v>3551</v>
       </c>
@@ -65472,7 +65548,9 @@
       <c r="C1663">
         <v>105</v>
       </c>
-      <c r="G1663" s="8"/>
+      <c r="G1663" s="14" t="s">
+        <v>5080</v>
+      </c>
       <c r="H1663" t="s">
         <v>3554</v>
       </c>
@@ -65499,7 +65577,9 @@
       <c r="C1664">
         <v>317</v>
       </c>
-      <c r="G1664" s="8"/>
+      <c r="G1664" s="14" t="s">
+        <v>5081</v>
+      </c>
       <c r="H1664" t="s">
         <v>4170</v>
       </c>
@@ -65526,7 +65606,9 @@
       <c r="C1665">
         <v>320</v>
       </c>
-      <c r="G1665" s="8"/>
+      <c r="G1665" s="14" t="s">
+        <v>5083</v>
+      </c>
       <c r="H1665" t="s">
         <v>4177</v>
       </c>
@@ -65553,7 +65635,9 @@
       <c r="C1666">
         <v>324</v>
       </c>
-      <c r="G1666" s="8"/>
+      <c r="G1666" s="14" t="s">
+        <v>5082</v>
+      </c>
       <c r="H1666" t="s">
         <v>4185</v>
       </c>
@@ -65580,7 +65664,9 @@
       <c r="C1667">
         <v>360</v>
       </c>
-      <c r="G1667" s="8"/>
+      <c r="G1667" s="14" t="s">
+        <v>442</v>
+      </c>
       <c r="H1667" t="s">
         <v>4276</v>
       </c>
@@ -65607,7 +65693,9 @@
       <c r="C1668">
         <v>370</v>
       </c>
-      <c r="G1668" s="8"/>
+      <c r="G1668" s="15" t="s">
+        <v>5078</v>
+      </c>
       <c r="H1668" t="s">
         <v>4302</v>
       </c>
@@ -65634,7 +65722,9 @@
       <c r="C1669">
         <v>376</v>
       </c>
-      <c r="G1669" s="8"/>
+      <c r="G1669" s="14" t="s">
+        <v>524</v>
+      </c>
       <c r="H1669" t="s">
         <v>3258</v>
       </c>
@@ -65665,9 +65755,11 @@
     <hyperlink ref="G1568" r:id="rId6" xr:uid="{E7D8909C-5532-497D-AFA8-FE463C7FA78C}"/>
     <hyperlink ref="G1576" r:id="rId7" xr:uid="{D09720F0-BC5B-4438-9DA7-16D025CC8254}"/>
     <hyperlink ref="G1593" r:id="rId8" xr:uid="{E471ACAE-6B3C-4097-ABF7-F9DCFF37593D}"/>
+    <hyperlink ref="G1657" r:id="rId9" xr:uid="{4D6A6305-9C7C-4B40-B016-31CFE0F74BFA}"/>
+    <hyperlink ref="G1668" r:id="rId10" xr:uid="{47F24428-0452-4B5A-A1F7-4522803A2F9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>